<commit_message>
Make excel file editable
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\MishraTeam\Research\Projects\MathModeling\Covid_model\time series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\David\Work\smh\COVID-19\covid-GTA-surge-planning-reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E038F-51DB-4CE2-93C4-6DA8D3EFDF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11355" windowHeight="8415"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,16 @@
     <sheet name="References" sheetId="2" r:id="rId3"/>
     <sheet name="Recommended Citation" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -122,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,7 +230,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -282,7 +295,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -341,7 +360,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9"/>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -400,7 +425,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -459,7 +490,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -518,7 +555,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -577,7 +620,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Rectangle 14"/>
+        <xdr:cNvPr id="15" name="Rectangle 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -636,7 +685,13 @@
     <xdr:ext cx="3153826" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -705,7 +760,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1793,7 +1854,13 @@
     <xdr:ext cx="11911291" cy="4585101"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2125,22 +2192,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:HW18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="BP2" sqref="BP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2835,7 +2902,7 @@
         <v>44084</v>
       </c>
     </row>
-    <row r="2" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3038,7 +3105,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="3" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:231" x14ac:dyDescent="0.3">
       <c r="AP3" s="8"/>
       <c r="AQ3" s="8"/>
       <c r="AR3" s="8"/>
@@ -3061,7 +3128,7 @@
       <c r="BI3" s="8"/>
       <c r="BJ3" s="8"/>
     </row>
-    <row r="4" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3195,10 +3262,10 @@
       </c>
       <c r="BP4" s="8"/>
     </row>
-    <row r="5" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP5" s="8"/>
     </row>
-    <row r="6" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3310,10 +3377,10 @@
       </c>
       <c r="BP6" s="8"/>
     </row>
-    <row r="7" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="8"/>
     </row>
-    <row r="8" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3437,10 +3504,10 @@
       </c>
       <c r="BP8" s="8"/>
     </row>
-    <row r="9" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="8"/>
     </row>
-    <row r="10" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -3578,7 +3645,7 @@
       </c>
       <c r="BP10" s="8"/>
     </row>
-    <row r="12" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3847,27 +3914,27 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="14" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:231" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -3883,16 +3950,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
     </row>
   </sheetData>
@@ -3902,29 +3969,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3932,12 +3999,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3945,7 +4012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3953,7 +4020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -3961,7 +4028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3969,12 +4036,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3982,7 +4049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -3996,21 +4063,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>

</xml_diff>